<commit_message>
Added tests and some fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganga\eclipse-workspace\seleniummaven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39446E7D-6FD9-4EB6-ABC1-5A70EC82854A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171383D2-6BB1-476B-A413-C415CD736C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
   <si>
     <t xml:space="preserve">login </t>
   </si>
@@ -43,13 +44,37 @@
   </si>
   <si>
     <t>B.S in Business Administration</t>
+  </si>
+  <si>
+    <t>B.S. in Criminal Justice</t>
+  </si>
+  <si>
+    <t>B.S in Public Health - Healthcare Management</t>
+  </si>
+  <si>
+    <t>B.S. in Health Studies - General</t>
+  </si>
+  <si>
+    <t>October 5th, 2020</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>M.S in Nursing</t>
+  </si>
+  <si>
+    <t>MS in Early Childhood Studies</t>
+  </si>
+  <si>
+    <t>B.S. in Health Studies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +82,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,13 +113,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,35 +419,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677FCC7C-D3F7-4D52-B8AD-E91C888C83B1}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More changes to the new scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganga\eclipse-workspace\seleniummaven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA6AFF9-2639-4752-84C6-798E2EDB316B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC4399D-0D30-4CBD-8753-6E0E95730D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +95,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,18 +146,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -632,10 +643,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677FCC7C-D3F7-4D52-B8AD-E91C888C83B1}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +684,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -687,34 +698,10 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{59A09571-16B3-448C-9060-FA35C85129B0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New fixes to testng.xml and pom.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganga\eclipse-workspace\seleniummaven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4D097B-348D-4357-948D-531C7034E388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BB2D1D-8CAB-42AE-AD63-50D500A0491D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
   <si>
     <t xml:space="preserve">login </t>
   </si>
@@ -65,6 +66,9 @@
   </si>
   <si>
     <t>Agile Scrum Master</t>
+  </si>
+  <si>
+    <t>surya.reddi@laureate.net.l1.l1qa2</t>
   </si>
 </sst>
 </file>
@@ -138,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -146,6 +150,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,7 +435,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,9 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677FCC7C-D3F7-4D52-B8AD-E91C888C83B1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -696,4 +699,53 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC92404-85F9-4D95-BB8E-8C42830C3025}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New test added l1
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganga\eclipse-workspace\seleniummaven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0446C5B0-F832-4C80-9706-669C37161C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E67D5D-3919-417D-924B-76FAA4D05A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
   <si>
     <t xml:space="preserve">login </t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Cloud Architect</t>
+  </si>
+  <si>
+    <t>StartDateName</t>
+  </si>
+  <si>
+    <t>uatlogin</t>
+  </si>
+  <si>
+    <t>suryakumar.reddi@laureate.net.cbl.uat</t>
+  </si>
+  <si>
+    <t>SD-228508</t>
   </si>
 </sst>
 </file>
@@ -142,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -150,7 +162,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677FCC7C-D3F7-4D52-B8AD-E91C888C83B1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,46 +695,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC92404-85F9-4D95-BB8E-8C42830C3025}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>